<commit_message>
Update everything (2021-02-24) but have added the daily .dta to gitignore
Former-commit-id: 334e5ee1a317ff6d1105f5b6661a6acde25c7ecb [formerly fdb3b4a68c53a624a6df214ba39db62d2924f7d2]

Former-commit-id: e0e88bf5d71829d34b8c27d4169ef88531d064f0
</commit_message>
<xml_diff>
--- a/USA Data/County level/Code book Dec 18.xlsx
+++ b/USA Data/County level/Code book Dec 18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isminiethridge/Dropbox/IE_COVID-19/2. US Data/County level/Masterfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isminiethridge/Dropbox/JDS_Data/USA Data/County level/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1611E50-6D2F-6143-A9B7-82A5D05A0995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AA69EC-0388-3245-A07F-954DA7EFC13D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1000" windowWidth="23200" windowHeight="16580" xr2:uid="{9AF4ABF2-81F0-8B45-91D6-996B43846C3C}"/>
+    <workbookView xWindow="3220" yWindow="460" windowWidth="23200" windowHeight="16580" xr2:uid="{9AF4ABF2-81F0-8B45-91D6-996B43846C3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Code book" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="989">
   <si>
     <t>ïfid</t>
   </si>
@@ -2962,6 +2962,39 @@
   </si>
   <si>
     <t>Number of establishments Wholesale trade2000</t>
+  </si>
+  <si>
+    <t>http://www.thearda.com/Archive/Files/Descriptions/RCMSCY10.asp</t>
+  </si>
+  <si>
+    <t>data retrieved from https://www.arcgis.com/home/item.html?id=8bc0305fac294c789844c49aaebe88ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Census Bureau </t>
+  </si>
+  <si>
+    <t>https://www.countyhealthrankings.org/</t>
+  </si>
+  <si>
+    <t>num_est</t>
+  </si>
+  <si>
+    <t>num_emp</t>
+  </si>
+  <si>
+    <t>pay_annual</t>
+  </si>
+  <si>
+    <t>number of establishments</t>
+  </si>
+  <si>
+    <t>number of employees</t>
+  </si>
+  <si>
+    <t>average annual pay</t>
+  </si>
+  <si>
+    <t>Suffix key</t>
   </si>
 </sst>
 </file>
@@ -3420,10 +3453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5495A087-993E-9D4C-90D9-606D55C44A57}">
-  <dimension ref="A1:E439"/>
+  <dimension ref="A1:E443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" topLeftCell="A422" workbookViewId="0">
+      <selection activeCell="C449" sqref="C449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5014,7 +5047,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>142</v>
       </c>
@@ -5025,250 +5058,385 @@
         <v>424</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>757</v>
       </c>
       <c r="B146" t="s">
         <v>784</v>
       </c>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C146" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D146" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>758</v>
       </c>
       <c r="B147" t="s">
         <v>785</v>
       </c>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C147" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D147" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>759</v>
       </c>
       <c r="B148" t="s">
         <v>786</v>
       </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C148" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D148" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>760</v>
       </c>
       <c r="B149" t="s">
         <v>788</v>
       </c>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C149" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D149" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>761</v>
       </c>
       <c r="B150" t="s">
         <v>789</v>
       </c>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C150" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D150" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>762</v>
       </c>
       <c r="B151" t="s">
         <v>790</v>
       </c>
-      <c r="C151"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C151" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D151" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>763</v>
       </c>
       <c r="B152" t="s">
         <v>791</v>
       </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C152" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D152" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>764</v>
       </c>
       <c r="B153" t="s">
         <v>792</v>
       </c>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C153" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D153" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>765</v>
       </c>
       <c r="B154" t="s">
         <v>793</v>
       </c>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C154" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D154" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>766</v>
       </c>
       <c r="B155" t="s">
         <v>794</v>
       </c>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C155" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D155" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>767</v>
       </c>
       <c r="B156" t="s">
         <v>795</v>
       </c>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C156" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D156" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>768</v>
       </c>
       <c r="B157" t="s">
         <v>796</v>
       </c>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C157" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D157" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>769</v>
       </c>
       <c r="B158" t="s">
         <v>797</v>
       </c>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C158" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D158" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>770</v>
       </c>
       <c r="B159" t="s">
         <v>798</v>
       </c>
-      <c r="C159"/>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C159" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D159" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>771</v>
       </c>
       <c r="B160" t="s">
         <v>799</v>
       </c>
-      <c r="C160"/>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C160" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D160" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>772</v>
       </c>
       <c r="B161" t="s">
         <v>800</v>
       </c>
-      <c r="C161"/>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C161" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D161" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>773</v>
       </c>
       <c r="B162" t="s">
         <v>801</v>
       </c>
-      <c r="C162"/>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C162" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D162" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>774</v>
       </c>
       <c r="B163" t="s">
         <v>802</v>
       </c>
-      <c r="C163"/>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C163" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D163" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>775</v>
       </c>
       <c r="B164" t="s">
         <v>803</v>
       </c>
-      <c r="C164"/>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C164" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D164" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>776</v>
       </c>
       <c r="B165" t="s">
         <v>804</v>
       </c>
-      <c r="C165"/>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C165" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D165" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>777</v>
       </c>
       <c r="B166" t="s">
         <v>805</v>
       </c>
-      <c r="C166"/>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C166" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D166" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>778</v>
       </c>
       <c r="B167" t="s">
         <v>806</v>
       </c>
-      <c r="C167"/>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C167" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D167" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>779</v>
       </c>
       <c r="B168" t="s">
         <v>807</v>
       </c>
-      <c r="C168"/>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C168" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D168" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>780</v>
       </c>
       <c r="B169" t="s">
         <v>808</v>
       </c>
-      <c r="C169"/>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C169" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D169" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>781</v>
       </c>
       <c r="B170" t="s">
         <v>809</v>
       </c>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C170" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D170" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>782</v>
       </c>
       <c r="B171" t="s">
         <v>787</v>
       </c>
-      <c r="C171"/>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C171" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D171" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>783</v>
       </c>
       <c r="B172" t="s">
         <v>810</v>
       </c>
-      <c r="C172"/>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C172" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D172" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>143</v>
       </c>
@@ -5279,7 +5447,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>168</v>
       </c>
@@ -5290,7 +5458,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>169</v>
       </c>
@@ -5301,7 +5469,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>170</v>
       </c>
@@ -6672,6 +6840,9 @@
       <c r="A300" t="s">
         <v>637</v>
       </c>
+      <c r="C300" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E300" t="s">
         <v>815</v>
       </c>
@@ -6680,6 +6851,9 @@
       <c r="A301" t="s">
         <v>638</v>
       </c>
+      <c r="C301" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E301" t="s">
         <v>816</v>
       </c>
@@ -6688,6 +6862,9 @@
       <c r="A302" t="s">
         <v>639</v>
       </c>
+      <c r="C302" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E302" t="s">
         <v>817</v>
       </c>
@@ -6696,6 +6873,9 @@
       <c r="A303" t="s">
         <v>640</v>
       </c>
+      <c r="C303" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E303" t="s">
         <v>818</v>
       </c>
@@ -6704,6 +6884,9 @@
       <c r="A304" t="s">
         <v>641</v>
       </c>
+      <c r="C304" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E304" t="s">
         <v>819</v>
       </c>
@@ -6712,6 +6895,9 @@
       <c r="A305" t="s">
         <v>642</v>
       </c>
+      <c r="C305" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E305" t="s">
         <v>820</v>
       </c>
@@ -6720,6 +6906,9 @@
       <c r="A306" t="s">
         <v>643</v>
       </c>
+      <c r="C306" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E306" t="s">
         <v>821</v>
       </c>
@@ -6728,6 +6917,9 @@
       <c r="A307" t="s">
         <v>644</v>
       </c>
+      <c r="C307" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E307" t="s">
         <v>822</v>
       </c>
@@ -6736,6 +6928,9 @@
       <c r="A308" t="s">
         <v>645</v>
       </c>
+      <c r="C308" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E308" t="s">
         <v>823</v>
       </c>
@@ -6744,6 +6939,9 @@
       <c r="A309" t="s">
         <v>646</v>
       </c>
+      <c r="C309" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E309" t="s">
         <v>824</v>
       </c>
@@ -6752,6 +6950,9 @@
       <c r="A310" t="s">
         <v>647</v>
       </c>
+      <c r="C310" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E310" t="s">
         <v>825</v>
       </c>
@@ -6760,6 +6961,9 @@
       <c r="A311" t="s">
         <v>648</v>
       </c>
+      <c r="C311" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E311" t="s">
         <v>826</v>
       </c>
@@ -6768,6 +6972,9 @@
       <c r="A312" t="s">
         <v>649</v>
       </c>
+      <c r="C312" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E312" t="s">
         <v>827</v>
       </c>
@@ -6776,6 +6983,9 @@
       <c r="A313" t="s">
         <v>650</v>
       </c>
+      <c r="C313" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E313" t="s">
         <v>828</v>
       </c>
@@ -6784,6 +6994,9 @@
       <c r="A314" t="s">
         <v>651</v>
       </c>
+      <c r="C314" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E314" t="s">
         <v>829</v>
       </c>
@@ -6792,6 +7005,9 @@
       <c r="A315" t="s">
         <v>652</v>
       </c>
+      <c r="C315" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E315" t="s">
         <v>830</v>
       </c>
@@ -6800,6 +7016,9 @@
       <c r="A316" t="s">
         <v>653</v>
       </c>
+      <c r="C316" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E316" t="s">
         <v>831</v>
       </c>
@@ -6808,6 +7027,9 @@
       <c r="A317" t="s">
         <v>654</v>
       </c>
+      <c r="C317" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E317" t="s">
         <v>832</v>
       </c>
@@ -6816,6 +7038,9 @@
       <c r="A318" t="s">
         <v>655</v>
       </c>
+      <c r="C318" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E318" t="s">
         <v>833</v>
       </c>
@@ -6824,6 +7049,9 @@
       <c r="A319" t="s">
         <v>656</v>
       </c>
+      <c r="C319" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E319" t="s">
         <v>834</v>
       </c>
@@ -6832,6 +7060,9 @@
       <c r="A320" t="s">
         <v>657</v>
       </c>
+      <c r="C320" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E320" t="s">
         <v>835</v>
       </c>
@@ -6840,6 +7071,9 @@
       <c r="A321" t="s">
         <v>658</v>
       </c>
+      <c r="C321" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E321" t="s">
         <v>836</v>
       </c>
@@ -6848,6 +7082,9 @@
       <c r="A322" t="s">
         <v>659</v>
       </c>
+      <c r="C322" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E322" t="s">
         <v>837</v>
       </c>
@@ -6856,6 +7093,9 @@
       <c r="A323" t="s">
         <v>660</v>
       </c>
+      <c r="C323" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E323" t="s">
         <v>838</v>
       </c>
@@ -6864,6 +7104,9 @@
       <c r="A324" t="s">
         <v>661</v>
       </c>
+      <c r="C324" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E324" t="s">
         <v>839</v>
       </c>
@@ -6872,6 +7115,9 @@
       <c r="A325" t="s">
         <v>662</v>
       </c>
+      <c r="C325" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E325" t="s">
         <v>840</v>
       </c>
@@ -6880,6 +7126,9 @@
       <c r="A326" t="s">
         <v>663</v>
       </c>
+      <c r="C326" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E326" t="s">
         <v>841</v>
       </c>
@@ -6888,6 +7137,9 @@
       <c r="A327" t="s">
         <v>664</v>
       </c>
+      <c r="C327" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E327" t="s">
         <v>842</v>
       </c>
@@ -6896,6 +7148,9 @@
       <c r="A328" t="s">
         <v>665</v>
       </c>
+      <c r="C328" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E328" t="s">
         <v>843</v>
       </c>
@@ -6904,6 +7159,9 @@
       <c r="A329" t="s">
         <v>666</v>
       </c>
+      <c r="C329" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E329" t="s">
         <v>844</v>
       </c>
@@ -6912,6 +7170,9 @@
       <c r="A330" t="s">
         <v>667</v>
       </c>
+      <c r="C330" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E330" t="s">
         <v>845</v>
       </c>
@@ -6920,6 +7181,9 @@
       <c r="A331" t="s">
         <v>668</v>
       </c>
+      <c r="C331" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E331" t="s">
         <v>846</v>
       </c>
@@ -6928,6 +7192,9 @@
       <c r="A332" t="s">
         <v>669</v>
       </c>
+      <c r="C332" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E332" t="s">
         <v>847</v>
       </c>
@@ -6936,6 +7203,9 @@
       <c r="A333" t="s">
         <v>670</v>
       </c>
+      <c r="C333" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E333" t="s">
         <v>848</v>
       </c>
@@ -6944,6 +7214,9 @@
       <c r="A334" t="s">
         <v>671</v>
       </c>
+      <c r="C334" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E334" t="s">
         <v>849</v>
       </c>
@@ -6952,6 +7225,9 @@
       <c r="A335" t="s">
         <v>672</v>
       </c>
+      <c r="C335" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E335" t="s">
         <v>850</v>
       </c>
@@ -6960,6 +7236,9 @@
       <c r="A336" t="s">
         <v>673</v>
       </c>
+      <c r="C336" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E336" t="s">
         <v>851</v>
       </c>
@@ -6968,6 +7247,9 @@
       <c r="A337" t="s">
         <v>674</v>
       </c>
+      <c r="C337" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E337" t="s">
         <v>852</v>
       </c>
@@ -6976,6 +7258,9 @@
       <c r="A338" t="s">
         <v>675</v>
       </c>
+      <c r="C338" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E338" t="s">
         <v>853</v>
       </c>
@@ -6984,6 +7269,9 @@
       <c r="A339" t="s">
         <v>676</v>
       </c>
+      <c r="C339" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E339" t="s">
         <v>854</v>
       </c>
@@ -6992,6 +7280,9 @@
       <c r="A340" t="s">
         <v>677</v>
       </c>
+      <c r="C340" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E340" t="s">
         <v>855</v>
       </c>
@@ -7000,6 +7291,9 @@
       <c r="A341" t="s">
         <v>678</v>
       </c>
+      <c r="C341" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E341" t="s">
         <v>856</v>
       </c>
@@ -7008,6 +7302,9 @@
       <c r="A342" t="s">
         <v>679</v>
       </c>
+      <c r="C342" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E342" t="s">
         <v>857</v>
       </c>
@@ -7016,6 +7313,9 @@
       <c r="A343" t="s">
         <v>680</v>
       </c>
+      <c r="C343" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E343" t="s">
         <v>858</v>
       </c>
@@ -7024,6 +7324,9 @@
       <c r="A344" t="s">
         <v>681</v>
       </c>
+      <c r="C344" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E344" t="s">
         <v>859</v>
       </c>
@@ -7032,6 +7335,9 @@
       <c r="A345" t="s">
         <v>682</v>
       </c>
+      <c r="C345" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E345" t="s">
         <v>860</v>
       </c>
@@ -7040,6 +7346,9 @@
       <c r="A346" t="s">
         <v>683</v>
       </c>
+      <c r="C346" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E346" t="s">
         <v>861</v>
       </c>
@@ -7048,6 +7357,9 @@
       <c r="A347" t="s">
         <v>684</v>
       </c>
+      <c r="C347" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E347" t="s">
         <v>862</v>
       </c>
@@ -7056,6 +7368,9 @@
       <c r="A348" t="s">
         <v>685</v>
       </c>
+      <c r="C348" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E348" t="s">
         <v>863</v>
       </c>
@@ -7064,6 +7379,9 @@
       <c r="A349" t="s">
         <v>686</v>
       </c>
+      <c r="C349" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E349" t="s">
         <v>864</v>
       </c>
@@ -7072,6 +7390,9 @@
       <c r="A350" t="s">
         <v>687</v>
       </c>
+      <c r="C350" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E350" t="s">
         <v>865</v>
       </c>
@@ -7080,6 +7401,9 @@
       <c r="A351" t="s">
         <v>688</v>
       </c>
+      <c r="C351" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E351" t="s">
         <v>866</v>
       </c>
@@ -7088,6 +7412,9 @@
       <c r="A352" t="s">
         <v>689</v>
       </c>
+      <c r="C352" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E352" t="s">
         <v>867</v>
       </c>
@@ -7096,6 +7423,9 @@
       <c r="A353" t="s">
         <v>690</v>
       </c>
+      <c r="C353" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E353" t="s">
         <v>868</v>
       </c>
@@ -7104,6 +7434,9 @@
       <c r="A354" t="s">
         <v>691</v>
       </c>
+      <c r="C354" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E354" t="s">
         <v>869</v>
       </c>
@@ -7112,6 +7445,9 @@
       <c r="A355" t="s">
         <v>692</v>
       </c>
+      <c r="C355" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E355" t="s">
         <v>870</v>
       </c>
@@ -7120,6 +7456,9 @@
       <c r="A356" t="s">
         <v>693</v>
       </c>
+      <c r="C356" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E356" t="s">
         <v>871</v>
       </c>
@@ -7128,6 +7467,9 @@
       <c r="A357" t="s">
         <v>694</v>
       </c>
+      <c r="C357" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E357" t="s">
         <v>872</v>
       </c>
@@ -7136,6 +7478,9 @@
       <c r="A358" t="s">
         <v>695</v>
       </c>
+      <c r="C358" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E358" t="s">
         <v>873</v>
       </c>
@@ -7144,6 +7489,9 @@
       <c r="A359" t="s">
         <v>696</v>
       </c>
+      <c r="C359" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="E359" t="s">
         <v>874</v>
       </c>
@@ -7635,6 +7983,9 @@
       <c r="B420" s="22" t="s">
         <v>534</v>
       </c>
+      <c r="C420" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
@@ -7643,6 +7994,9 @@
       <c r="B421" s="22" t="s">
         <v>535</v>
       </c>
+      <c r="C421" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
@@ -7651,6 +8005,9 @@
       <c r="B422" s="22" t="s">
         <v>536</v>
       </c>
+      <c r="C422" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
@@ -7659,6 +8016,9 @@
       <c r="B423" s="22" t="s">
         <v>537</v>
       </c>
+      <c r="C423" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
@@ -7667,6 +8027,9 @@
       <c r="B424" s="22" t="s">
         <v>538</v>
       </c>
+      <c r="C424" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
@@ -7675,6 +8038,9 @@
       <c r="B425" s="22" t="s">
         <v>539</v>
       </c>
+      <c r="C425" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
@@ -7683,6 +8049,9 @@
       <c r="B426" s="22" t="s">
         <v>540</v>
       </c>
+      <c r="C426" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
@@ -7691,6 +8060,9 @@
       <c r="B427" s="22" t="s">
         <v>541</v>
       </c>
+      <c r="C427" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
@@ -7699,6 +8071,9 @@
       <c r="B428" s="22" t="s">
         <v>542</v>
       </c>
+      <c r="C428" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
@@ -7707,6 +8082,9 @@
       <c r="B429" s="22" t="s">
         <v>543</v>
       </c>
+      <c r="C429" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
@@ -7715,6 +8093,9 @@
       <c r="B430" s="22" t="s">
         <v>544</v>
       </c>
+      <c r="C430" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
@@ -7723,6 +8104,9 @@
       <c r="B431" s="22" t="s">
         <v>545</v>
       </c>
+      <c r="C431" s="18" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
@@ -7731,34 +8115,43 @@
       <c r="B432" s="22" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C432" s="18" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>532</v>
       </c>
       <c r="B433" s="22" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C433" s="18" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>533</v>
       </c>
       <c r="B434" s="22" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C434" s="18" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>331</v>
       </c>
@@ -7766,7 +8159,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>332</v>
       </c>
@@ -7774,12 +8167,44 @@
         <v>334</v>
       </c>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>936</v>
       </c>
       <c r="B439" t="s">
         <v>937</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A440" t="s">
+        <v>518</v>
+      </c>
+      <c r="C440" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A441" t="s">
+        <v>516</v>
+      </c>
+      <c r="C441" s="2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A442" t="s">
+        <v>636</v>
+      </c>
+      <c r="C442" s="2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A443" t="s">
+        <v>517</v>
+      </c>
+      <c r="C443" s="2" t="s">
+        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -7798,6 +8223,12 @@
     <hyperlink ref="C237" r:id="rId11" xr:uid="{ABD24312-7BF6-2647-888A-2B84FFF93C6E}"/>
     <hyperlink ref="C238:C299" r:id="rId12" display="U.S. Census Bureau, 2000 County Business Patterns&lt;br&gt;" xr:uid="{006F795B-9A7D-3B4C-86BD-0402A4A982B6}"/>
     <hyperlink ref="E299" r:id="rId13" xr:uid="{FBFA6698-72BC-4C4B-A726-EEFEBCCFC16C}"/>
+    <hyperlink ref="C146" r:id="rId14" xr:uid="{34112340-EC85-B648-BAF8-AD59623B22F5}"/>
+    <hyperlink ref="C147:C162" r:id="rId15" display="http://www.thearda.com/Archive/Files/Descriptions/RCMSCY10.asp" xr:uid="{70DEB881-2F23-0643-8161-06DBE617A298}"/>
+    <hyperlink ref="C163:C172" r:id="rId16" display="http://www.thearda.com/Archive/Files/Descriptions/RCMSCY10.asp" xr:uid="{3105E7EF-F210-AB43-93C5-323240BDFEBA}"/>
+    <hyperlink ref="C441" r:id="rId17" xr:uid="{33C3F498-8151-A24F-AC56-E8597C7C8C53}"/>
+    <hyperlink ref="C442" r:id="rId18" xr:uid="{79625A4A-086E-174C-A176-90561622E8AA}"/>
+    <hyperlink ref="C443" r:id="rId19" xr:uid="{98FAB613-9DEA-C64A-8FFD-45788AFDC4CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7805,19 +8236,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC83901C-D10E-9947-BBB7-9C69F191B5E4}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>338</v>
       </c>
@@ -7827,8 +8259,11 @@
       <c r="C1" s="1" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -7839,7 +8274,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -7850,7 +8285,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -7861,7 +8296,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -7872,7 +8307,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -7883,7 +8318,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -7894,7 +8329,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -7905,7 +8340,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -7916,7 +8351,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -7927,7 +8362,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -7938,7 +8373,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -7949,7 +8384,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -7960,7 +8395,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>159</v>
       </c>
@@ -7971,7 +8406,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -7982,7 +8417,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -8054,6 +8489,35 @@
       </c>
       <c r="B22" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>982</v>
+      </c>
+      <c r="B25" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>983</v>
+      </c>
+      <c r="B26" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>984</v>
+      </c>
+      <c r="B27" t="s">
+        <v>987</v>
       </c>
     </row>
   </sheetData>
@@ -8398,10 +8862,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A909EBA-CC36-5C4D-9FCC-8AAF6A9B9674}">
-  <dimension ref="A1:C124"/>
+  <dimension ref="A4:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8411,24 +8875,6 @@
     <col min="3" max="3" width="61.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>636</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>517</v>
@@ -8437,970 +8883,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>637</v>
-      </c>
-      <c r="C5" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>638</v>
-      </c>
-      <c r="C6" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>639</v>
-      </c>
-      <c r="C7" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>640</v>
-      </c>
-      <c r="C8" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>641</v>
-      </c>
-      <c r="C9" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>642</v>
-      </c>
-      <c r="C10" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>643</v>
-      </c>
-      <c r="C11" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>644</v>
-      </c>
-      <c r="C12" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>645</v>
-      </c>
-      <c r="C13" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>646</v>
-      </c>
-      <c r="C14" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>647</v>
-      </c>
-      <c r="C15" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>648</v>
-      </c>
-      <c r="C16" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>649</v>
-      </c>
-      <c r="C17" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>650</v>
-      </c>
-      <c r="C18" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>651</v>
-      </c>
-      <c r="C19" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>652</v>
-      </c>
-      <c r="C20" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>653</v>
-      </c>
-      <c r="C21" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>654</v>
-      </c>
-      <c r="C22" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>655</v>
-      </c>
-      <c r="C23" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>656</v>
-      </c>
-      <c r="C24" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>657</v>
-      </c>
-      <c r="C25" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>658</v>
-      </c>
-      <c r="C26" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>659</v>
-      </c>
-      <c r="C27" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>660</v>
-      </c>
-      <c r="C28" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>661</v>
-      </c>
-      <c r="C29" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>662</v>
-      </c>
-      <c r="C30" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>663</v>
-      </c>
-      <c r="C31" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>664</v>
-      </c>
-      <c r="C32" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>665</v>
-      </c>
-      <c r="C33" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>666</v>
-      </c>
-      <c r="C34" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>667</v>
-      </c>
-      <c r="C35" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>668</v>
-      </c>
-      <c r="C36" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>669</v>
-      </c>
-      <c r="C37" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>670</v>
-      </c>
-      <c r="C38" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>671</v>
-      </c>
-      <c r="C39" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>672</v>
-      </c>
-      <c r="C40" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>673</v>
-      </c>
-      <c r="C41" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>674</v>
-      </c>
-      <c r="C42" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>675</v>
-      </c>
-      <c r="C43" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>676</v>
-      </c>
-      <c r="C44" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>677</v>
-      </c>
-      <c r="C45" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>678</v>
-      </c>
-      <c r="C46" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>679</v>
-      </c>
-      <c r="C47" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>680</v>
-      </c>
-      <c r="C48" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>681</v>
-      </c>
-      <c r="C49" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>682</v>
-      </c>
-      <c r="C50" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>683</v>
-      </c>
-      <c r="C51" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>684</v>
-      </c>
-      <c r="C52" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>685</v>
-      </c>
-      <c r="C53" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>686</v>
-      </c>
-      <c r="C54" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>687</v>
-      </c>
-      <c r="C55" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>688</v>
-      </c>
-      <c r="C56" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>689</v>
-      </c>
-      <c r="C57" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>690</v>
-      </c>
-      <c r="C58" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>691</v>
-      </c>
-      <c r="C59" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>692</v>
-      </c>
-      <c r="C60" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>693</v>
-      </c>
-      <c r="C61" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>694</v>
-      </c>
-      <c r="C62" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>695</v>
-      </c>
-      <c r="C63" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>696</v>
-      </c>
-      <c r="C64" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>697</v>
-      </c>
-      <c r="C65" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>698</v>
-      </c>
-      <c r="C66" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>699</v>
-      </c>
-      <c r="C67" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>700</v>
-      </c>
-      <c r="C68" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>701</v>
-      </c>
-      <c r="C69" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>702</v>
-      </c>
-      <c r="C70" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>703</v>
-      </c>
-      <c r="C71" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>704</v>
-      </c>
-      <c r="C72" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>705</v>
-      </c>
-      <c r="C73" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>706</v>
-      </c>
-      <c r="C74" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>707</v>
-      </c>
-      <c r="C75" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>708</v>
-      </c>
-      <c r="C76" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>709</v>
-      </c>
-      <c r="C77" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>710</v>
-      </c>
-      <c r="C78" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>711</v>
-      </c>
-      <c r="C79" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>712</v>
-      </c>
-      <c r="C80" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>713</v>
-      </c>
-      <c r="C81" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>714</v>
-      </c>
-      <c r="C82" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>715</v>
-      </c>
-      <c r="C83" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>716</v>
-      </c>
-      <c r="C84" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>717</v>
-      </c>
-      <c r="C85" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>718</v>
-      </c>
-      <c r="C86" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>719</v>
-      </c>
-      <c r="C87" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>720</v>
-      </c>
-      <c r="C88" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>721</v>
-      </c>
-      <c r="C89" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>722</v>
-      </c>
-      <c r="C90" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>723</v>
-      </c>
-      <c r="C91" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>724</v>
-      </c>
-      <c r="C92" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>725</v>
-      </c>
-      <c r="C93" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>726</v>
-      </c>
-      <c r="C94" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>727</v>
-      </c>
-      <c r="C95" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>728</v>
-      </c>
-      <c r="C96" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>729</v>
-      </c>
-      <c r="C97" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>730</v>
-      </c>
-      <c r="C98" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>731</v>
-      </c>
-      <c r="C99" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>732</v>
-      </c>
-      <c r="C100" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>733</v>
-      </c>
-      <c r="C101" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>734</v>
-      </c>
-      <c r="C102" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>735</v>
-      </c>
-      <c r="C103" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>736</v>
-      </c>
-      <c r="C104" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>737</v>
-      </c>
-      <c r="C105" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>738</v>
-      </c>
-      <c r="C106" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>739</v>
-      </c>
-      <c r="C107" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>740</v>
-      </c>
-      <c r="C108" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>741</v>
-      </c>
-      <c r="C109" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>742</v>
-      </c>
-      <c r="C110" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>743</v>
-      </c>
-      <c r="C111" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>744</v>
-      </c>
-      <c r="C112" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>745</v>
-      </c>
-      <c r="C113" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>746</v>
-      </c>
-      <c r="C114" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>747</v>
-      </c>
-      <c r="C115" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>748</v>
-      </c>
-      <c r="C116" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>749</v>
-      </c>
-      <c r="C117" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>750</v>
-      </c>
-      <c r="C118" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>751</v>
-      </c>
-      <c r="C119" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>752</v>
-      </c>
-      <c r="C120" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>753</v>
-      </c>
-      <c r="C121" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>754</v>
-      </c>
-      <c r="C122" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>755</v>
-      </c>
-      <c r="C123" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>756</v>
-      </c>
-      <c r="C124" t="s">
-        <v>934</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{33C3F498-8151-A24F-AC56-E8597C7C8C53}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>